<commit_message>
Consultar detalle de facturas inscritas y programadas
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/ProgramarFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/ProgramarFacturas.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\administrarfacturas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31148B8-33B6-4705-B5F9-EF1CDA26FFE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="3" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -80,7 +74,10 @@
     <t>numeroIntento</t>
   </si>
   <si>
-    <t>fechaInicioFin</t>
+    <t>FechaInicio</t>
+  </si>
+  <si>
+    <t>fechaFin</t>
   </si>
   <si>
     <t>mesProgramacion</t>
@@ -92,6 +89,9 @@
     <t>1</t>
   </si>
   <si>
+    <t>autotest11</t>
+  </si>
+  <si>
     <t>1234</t>
   </si>
   <si>
@@ -125,13 +125,16 @@
     <t>Vence 05 Abr 2020</t>
   </si>
   <si>
+    <t>406-166630-04</t>
+  </si>
+  <si>
     <t>Corriente</t>
   </si>
   <si>
     <t>En la fecha de vencimiento</t>
   </si>
   <si>
-    <t>7-9</t>
+    <t>9</t>
   </si>
   <si>
     <t>Septiembre</t>
@@ -186,19 +189,19 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>autotest11</t>
-  </si>
-  <si>
-    <t>406-166630-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,14 +225,158 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +401,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -291,12 +624,254 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -307,20 +882,64 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -578,26 +1197,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
-    <col min="13" max="13" width="12.08203125"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.0833333333333"/>
+    <col min="14" max="14" width="18.3333333333333" customWidth="1"/>
     <col min="15" max="15" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,165 +1280,174 @@
       <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4">
         <v>48346663</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="S2" s="3">
         <v>1</v>
       </c>
-      <c r="T2" s="9" t="s">
-        <v>36</v>
+      <c r="T2" s="3">
+        <v>7</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.58203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.5833333333333" customWidth="1"/>
+    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.0833333333333" customWidth="1"/>
+    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nuevos mapeos para el flujo programar facturas, falta ejecución
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/ProgramarFacturas.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/administrarfacturas/ProgramarFacturas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -89,7 +89,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>autotest11</t>
+    <t>recaudosnatik66</t>
   </si>
   <si>
     <t>1234</t>
@@ -119,9 +119,6 @@
     <t>55.700,07</t>
   </si>
   <si>
-    <t>FACTURANET01 - 65401</t>
-  </si>
-  <si>
     <t>05 Abr 2020</t>
   </si>
   <si>
@@ -134,7 +131,7 @@
     <t>En la fecha de vencimiento</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Octubre</t>
@@ -197,9 +194,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -239,55 +236,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,12 +269,27 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -333,9 +307,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -354,25 +350,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -403,49 +400,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,127 +550,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,21 +616,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -656,21 +638,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -716,152 +683,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1199,8 +1196,8 @@
   <sheetPr/>
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1321,35 +1318,35 @@
       <c r="M2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="3">
+        <v>65401</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="S2" s="3">
         <v>1</v>
       </c>
       <c r="T2" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1377,16 +1374,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1394,50 +1391,50 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>